<commit_message>
Fixing Lab 9 charts
</commit_message>
<xml_diff>
--- a/09_insulin_overdose/09_insulin_overdose_data.xlsx
+++ b/09_insulin_overdose/09_insulin_overdose_data.xlsx
@@ -195,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -220,45 +220,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -561,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
@@ -633,25 +608,25 @@
       <c r="T2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="10">
         <v>0.5</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="10">
         <v>0.25</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="10">
         <v>0.25694444444444448</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="10">
         <v>0.2638888888888889</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="10">
         <v>0.27083333333333331</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="10">
         <v>0.27777777777777779</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="10">
         <v>0.28472222222222221</v>
       </c>
     </row>
@@ -704,34 +679,34 @@
       <c r="R3" s="4">
         <v>18.7</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="10">
+      <c r="U3" s="11">
         <f>ABS((B3-L3)/B3)</f>
         <v>9.7087378640776344E-3</v>
       </c>
-      <c r="V3" s="10">
+      <c r="V3" s="11">
         <f t="shared" ref="V3:AA3" si="0">ABS((C3-M3)/C3)</f>
         <v>0.39259259259259266</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="11">
         <f t="shared" si="0"/>
         <v>0.82608695652173914</v>
       </c>
-      <c r="X3" s="10">
+      <c r="X3" s="11">
         <f t="shared" si="0"/>
         <v>0.87680209698558309</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="11">
         <f t="shared" si="0"/>
         <v>0.88992974238875877</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="Z3" s="11">
         <f t="shared" si="0"/>
         <v>0.89599555061179093</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AA3" s="11">
         <f t="shared" si="0"/>
         <v>0.89423076923076927</v>
       </c>
@@ -785,34 +760,34 @@
       <c r="R4" s="4">
         <v>71.400000000000006</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4" s="11">
         <f t="shared" ref="U4:U11" si="1">ABS((B4-L4)/B4)</f>
         <v>0.10649350649350653</v>
       </c>
-      <c r="V4" s="10">
+      <c r="V4" s="11">
         <f t="shared" ref="V4:V11" si="2">ABS((C4-M4)/C4)</f>
         <v>0.21868131868131874</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4" s="11">
         <f t="shared" ref="W4:W11" si="3">ABS((D4-N4)/D4)</f>
         <v>9.8734177215189831E-2</v>
       </c>
-      <c r="X4" s="10">
+      <c r="X4" s="11">
         <f t="shared" ref="X4:X11" si="4">ABS((E4-O4)/E4)</f>
         <v>4.7058823529411806E-2</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Y4" s="11">
         <f t="shared" ref="Y4:Y11" si="5">ABS((F4-P4)/F4)</f>
         <v>1.857142857142853E-2</v>
       </c>
-      <c r="Z4" s="10">
+      <c r="Z4" s="11">
         <f t="shared" ref="Z4:Z11" si="6">ABS((G4-Q4)/G4)</f>
         <v>0.11975308641975312</v>
       </c>
-      <c r="AA4" s="10">
+      <c r="AA4" s="11">
         <f t="shared" ref="AA4:AA11" si="7">ABS((H4-R4)/H4)</f>
         <v>7.2727272727272654E-2</v>
       </c>
@@ -866,34 +841,34 @@
       <c r="R5" s="4">
         <v>89.9</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="T5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="10">
+      <c r="U5" s="11">
         <f t="shared" si="1"/>
         <v>5.8878504672897167E-2</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="11">
         <f t="shared" si="2"/>
         <v>7.85714285714285E-2</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="11">
         <f t="shared" si="3"/>
         <v>0.17532467532467533</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="11">
         <f t="shared" si="4"/>
         <v>0.50666666666666671</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="11">
         <f t="shared" si="5"/>
         <v>1.5055555555555555</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5" s="11">
         <f t="shared" si="6"/>
         <v>2.6039999999999996</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5" s="11">
         <f t="shared" si="7"/>
         <v>6.4916666666666671</v>
       </c>
@@ -947,34 +922,34 @@
       <c r="R6" s="4">
         <v>48.3</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U6" s="10">
+      <c r="U6" s="11">
         <f t="shared" si="1"/>
         <v>0.15124555160142347</v>
       </c>
-      <c r="V6" s="10">
+      <c r="V6" s="11">
         <f t="shared" si="2"/>
         <v>0.12972972972972979</v>
       </c>
-      <c r="W6" s="10">
+      <c r="W6" s="11">
         <f t="shared" si="3"/>
         <v>0.13285457809694803</v>
       </c>
-      <c r="X6" s="10">
+      <c r="X6" s="11">
         <f t="shared" si="4"/>
         <v>2.0661157024793684E-3</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Y6" s="11">
         <f t="shared" si="5"/>
         <v>0.58360655737704914</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="Z6" s="11">
         <f t="shared" si="6"/>
         <v>1.2890995260663505</v>
       </c>
-      <c r="AA6" s="10"/>
+      <c r="AA6" s="11"/>
     </row>
     <row r="7" spans="1:27" ht="60.75" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -1025,34 +1000,34 @@
       <c r="R7" s="4">
         <v>1.76</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="T7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U7" s="10">
+      <c r="U7" s="11">
         <f t="shared" si="1"/>
         <v>0.73636363636363611</v>
       </c>
-      <c r="V7" s="10">
+      <c r="V7" s="11">
         <f t="shared" si="2"/>
         <v>0.18000000000000002</v>
       </c>
-      <c r="W7" s="10">
+      <c r="W7" s="11">
         <f t="shared" si="3"/>
         <v>0.2642857142857144</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="11">
         <f t="shared" si="4"/>
         <v>0.47500000000000009</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="11">
         <f t="shared" si="5"/>
         <v>0.25714285714285723</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="Z7" s="11">
         <f t="shared" si="6"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="AA7" s="10"/>
+      <c r="AA7" s="11"/>
     </row>
     <row r="8" spans="1:27" ht="60.75" thickBot="1">
       <c r="A8" s="3" t="s">
@@ -1103,16 +1078,16 @@
       <c r="R8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="T8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
     </row>
     <row r="9" spans="1:27" ht="45.75" thickBot="1">
       <c r="A9" s="3" t="s">
@@ -1163,34 +1138,34 @@
       <c r="R9" s="4">
         <v>72</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="T9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U9" s="10">
+      <c r="U9" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X9" s="10">
+      <c r="X9" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="11">
         <f t="shared" si="5"/>
         <v>0.4375</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="Z9" s="11">
         <f t="shared" si="6"/>
         <v>0.4375</v>
       </c>
-      <c r="AA9" s="10"/>
+      <c r="AA9" s="11"/>
     </row>
     <row r="10" spans="1:27" ht="45.75" thickBot="1">
       <c r="A10" s="3" t="s">
@@ -1241,16 +1216,16 @@
       <c r="R10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="T10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
     </row>
     <row r="11" spans="1:27" ht="60.75" thickBot="1">
       <c r="A11" s="3" t="s">
@@ -1301,34 +1276,34 @@
       <c r="R11" s="4">
         <v>1.5</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="T11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U11" s="10">
+      <c r="U11" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V11" s="10">
+      <c r="V11" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W11" s="10">
+      <c r="W11" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X11" s="10">
+      <c r="X11" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="Y11" s="11">
         <f t="shared" si="5"/>
         <v>0.6875</v>
       </c>
-      <c r="Z11" s="10">
+      <c r="Z11" s="11">
         <f t="shared" si="6"/>
         <v>0.68085106382978722</v>
       </c>
-      <c r="AA11" s="10">
+      <c r="AA11" s="11">
         <f t="shared" si="7"/>
         <v>0.82352941176470584</v>
       </c>
@@ -1346,11 +1321,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="U3:AA11">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>